<commit_message>
util variance excel workbook
</commit_message>
<xml_diff>
--- a/operationalizedsamplingplans/csv_utility/utilevals_BASE (VARIANCE EVALUATION).xlsx
+++ b/operationalizedsamplingplans/csv_utility/utilevals_BASE (VARIANCE EVALUATION).xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Repositories\logistigateanalysis\operationalizedsamplingplans\csv_utility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\OneDrive\Documents\EAGER Project\Simulator\logistigateanalysis\operationalizedsamplingplans\csv_utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED50B53-9284-47E5-861E-FE8DADE17BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3647BEC4-454B-4BDD-BDA9-BECC5A9A6E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="345" windowWidth="21390" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="utilevals_BASE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5003,6 +5002,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Utility</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> estimates for 81 tests at select districts</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5061,10 +5090,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:srgbClr val="00B050"/>
                 </a:solidFill>
@@ -5179,10 +5208,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
@@ -5297,10 +5326,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:srgbClr val="FFC000"/>
                 </a:solidFill>
@@ -5415,10 +5444,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:srgbClr val="FFC000"/>
                 </a:solidFill>
@@ -5533,10 +5562,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="accent5">
                     <a:lumMod val="60000"/>
@@ -5654,10 +5683,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="accent5">
                     <a:lumMod val="60000"/>
@@ -5775,10 +5804,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -5855,10 +5884,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525">
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -7262,10 +7291,10 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7614,8 +7643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8013,11 +8042,11 @@
         <v>219</v>
       </c>
       <c r="S4" s="2">
-        <f t="shared" ref="S3:S47" si="14">_xlfn.NUMBERVALUE(_xlfn.TEXTAFTER(_xlfn.TEXTBEFORE(R4,","),"("))</f>
+        <f t="shared" ref="S4:S47" si="14">_xlfn.NUMBERVALUE(_xlfn.TEXTAFTER(_xlfn.TEXTBEFORE(R4,","),"("))</f>
         <v>0.29448841388254299</v>
       </c>
       <c r="T4" s="2">
-        <f t="shared" ref="T3:T47" si="15">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(R4,","),")"))</f>
+        <f t="shared" ref="T4:T47" si="15">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(R4,","),")"))</f>
         <v>0.30741893399816</v>
       </c>
       <c r="U4" s="2">

</xml_diff>